<commit_message>
removed excess sheets from some excel files
</commit_message>
<xml_diff>
--- a/data/Study 7/raw/extinction/intention_ratings_1_3.xlsx
+++ b/data/Study 7/raw/extinction/intention_ratings_1_3.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10413"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sean\Desktop\Office Laptop Files\1. Research Files\64. SH SM JDH (IR, Extinction, Counter)\2. Raw Data\Study 4 (Extinction Both Outcomes Mouse)\Extinction Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ian/git/intersecting_regularities_counter_conditioning/data/Study 7/raw/extinction/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C57BAEB3-08A2-6148-BF8A-50F0A28D60ED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10800" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="10800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inquisit Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="133">
   <si>
     <t>date</t>
   </si>
@@ -419,15 +419,12 @@
   </si>
   <si>
     <t>12:00:40</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1227,16 +1224,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H120"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C13" sqref="A1:H120"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1262,7 +1259,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>62017</v>
       </c>
@@ -1288,7 +1285,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>62017</v>
       </c>
@@ -1314,7 +1311,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>62017</v>
       </c>
@@ -1340,7 +1337,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>62017</v>
       </c>
@@ -1366,7 +1363,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>62017</v>
       </c>
@@ -1392,7 +1389,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>62017</v>
       </c>
@@ -1418,7 +1415,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>62017</v>
       </c>
@@ -1444,7 +1441,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>62017</v>
       </c>
@@ -1470,7 +1467,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>62017</v>
       </c>
@@ -1496,7 +1493,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>62017</v>
       </c>
@@ -1522,7 +1519,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>62017</v>
       </c>
@@ -1548,7 +1545,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>62017</v>
       </c>
@@ -1574,7 +1571,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>62017</v>
       </c>
@@ -1600,7 +1597,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>62017</v>
       </c>
@@ -1626,7 +1623,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>62017</v>
       </c>
@@ -1652,7 +1649,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>62017</v>
       </c>
@@ -1678,7 +1675,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>62017</v>
       </c>
@@ -1704,7 +1701,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>62017</v>
       </c>
@@ -1730,7 +1727,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>62017</v>
       </c>
@@ -1756,7 +1753,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>62017</v>
       </c>
@@ -1782,7 +1779,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>62017</v>
       </c>
@@ -1808,7 +1805,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>62117</v>
       </c>
@@ -1834,7 +1831,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>62117</v>
       </c>
@@ -1860,7 +1857,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>62117</v>
       </c>
@@ -1886,7 +1883,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>62117</v>
       </c>
@@ -1912,7 +1909,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>62117</v>
       </c>
@@ -1938,7 +1935,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>62117</v>
       </c>
@@ -1964,7 +1961,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>62117</v>
       </c>
@@ -1990,7 +1987,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>62117</v>
       </c>
@@ -2016,7 +2013,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>62117</v>
       </c>
@@ -2042,7 +2039,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>62117</v>
       </c>
@@ -2068,7 +2065,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>62117</v>
       </c>
@@ -2094,7 +2091,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>62117</v>
       </c>
@@ -2120,7 +2117,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>62117</v>
       </c>
@@ -2146,7 +2143,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>62117</v>
       </c>
@@ -2172,7 +2169,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>62117</v>
       </c>
@@ -2198,7 +2195,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>62117</v>
       </c>
@@ -2224,7 +2221,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>62117</v>
       </c>
@@ -2250,7 +2247,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>62117</v>
       </c>
@@ -2276,7 +2273,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>62117</v>
       </c>
@@ -2302,7 +2299,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>62117</v>
       </c>
@@ -2328,7 +2325,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>62117</v>
       </c>
@@ -2354,7 +2351,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>62117</v>
       </c>
@@ -2380,7 +2377,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>62117</v>
       </c>
@@ -2406,7 +2403,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>62117</v>
       </c>
@@ -2432,7 +2429,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>62117</v>
       </c>
@@ -2458,7 +2455,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>62117</v>
       </c>
@@ -2484,7 +2481,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>62117</v>
       </c>
@@ -2510,7 +2507,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>62117</v>
       </c>
@@ -2536,7 +2533,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>62117</v>
       </c>
@@ -2562,7 +2559,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>62117</v>
       </c>
@@ -2588,7 +2585,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>62117</v>
       </c>
@@ -2614,7 +2611,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>62117</v>
       </c>
@@ -2640,7 +2637,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>62117</v>
       </c>
@@ -2666,7 +2663,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>62117</v>
       </c>
@@ -2692,7 +2689,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>62117</v>
       </c>
@@ -2718,7 +2715,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>62117</v>
       </c>
@@ -2744,7 +2741,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>62117</v>
       </c>
@@ -2770,7 +2767,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>62117</v>
       </c>
@@ -2796,7 +2793,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>62117</v>
       </c>
@@ -2822,7 +2819,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>62117</v>
       </c>
@@ -2848,7 +2845,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62117</v>
       </c>
@@ -2874,7 +2871,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>62117</v>
       </c>
@@ -2900,7 +2897,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>62117</v>
       </c>
@@ -2926,7 +2923,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>62117</v>
       </c>
@@ -2952,7 +2949,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>62117</v>
       </c>
@@ -2978,7 +2975,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>62117</v>
       </c>
@@ -3004,7 +3001,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>62117</v>
       </c>
@@ -3030,7 +3027,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>62117</v>
       </c>
@@ -3056,7 +3053,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>62117</v>
       </c>
@@ -3082,7 +3079,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>62117</v>
       </c>
@@ -3108,7 +3105,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>62117</v>
       </c>
@@ -3134,7 +3131,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>62117</v>
       </c>
@@ -3160,7 +3157,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>62117</v>
       </c>
@@ -3186,7 +3183,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>62117</v>
       </c>
@@ -3212,7 +3209,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>62117</v>
       </c>
@@ -3238,7 +3235,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>62117</v>
       </c>
@@ -3264,7 +3261,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>62117</v>
       </c>
@@ -3290,7 +3287,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>62117</v>
       </c>
@@ -3316,7 +3313,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>62117</v>
       </c>
@@ -3342,7 +3339,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>62117</v>
       </c>
@@ -3368,7 +3365,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>62117</v>
       </c>
@@ -3394,7 +3391,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>62117</v>
       </c>
@@ -3420,7 +3417,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>62117</v>
       </c>
@@ -3446,7 +3443,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>62117</v>
       </c>
@@ -3472,7 +3469,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>62117</v>
       </c>
@@ -3498,7 +3495,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>62117</v>
       </c>
@@ -3524,7 +3521,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>62117</v>
       </c>
@@ -3550,7 +3547,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>62117</v>
       </c>
@@ -3576,7 +3573,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>62117</v>
       </c>
@@ -3602,7 +3599,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>62117</v>
       </c>
@@ -3628,7 +3625,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>62117</v>
       </c>
@@ -3654,7 +3651,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>62117</v>
       </c>
@@ -3680,7 +3677,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>62117</v>
       </c>
@@ -3706,7 +3703,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>62117</v>
       </c>
@@ -3732,7 +3729,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>62117</v>
       </c>
@@ -3758,7 +3755,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>62117</v>
       </c>
@@ -3784,7 +3781,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>62117</v>
       </c>
@@ -3810,7 +3807,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>62117</v>
       </c>
@@ -3836,7 +3833,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>62117</v>
       </c>
@@ -3862,7 +3859,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>62117</v>
       </c>
@@ -3888,7 +3885,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>62117</v>
       </c>
@@ -3914,7 +3911,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>62117</v>
       </c>
@@ -3940,7 +3937,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>62117</v>
       </c>
@@ -3966,7 +3963,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>62117</v>
       </c>
@@ -3992,7 +3989,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>62117</v>
       </c>
@@ -4018,7 +4015,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>62117</v>
       </c>
@@ -4044,7 +4041,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>62117</v>
       </c>
@@ -4070,7 +4067,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>62117</v>
       </c>
@@ -4096,7 +4093,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>62117</v>
       </c>
@@ -4122,7 +4119,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>62117</v>
       </c>
@@ -4148,7 +4145,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>62117</v>
       </c>
@@ -4174,7 +4171,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>62117</v>
       </c>
@@ -4200,7 +4197,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>62117</v>
       </c>
@@ -4226,7 +4223,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>62117</v>
       </c>
@@ -4252,7 +4249,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>62217</v>
       </c>
@@ -4278,7 +4275,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>62117</v>
       </c>
@@ -4304,7 +4301,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>62117</v>
       </c>
@@ -4330,7 +4327,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>62117</v>
       </c>
@@ -4359,1697 +4356,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D120"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C120"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>11</v>
-      </c>
-      <c r="B8">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>12</v>
-      </c>
-      <c r="B9">
-        <v>12</v>
-      </c>
-      <c r="C9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>15</v>
-      </c>
-      <c r="B10">
-        <v>15</v>
-      </c>
-      <c r="C10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>17</v>
-      </c>
-      <c r="B11">
-        <v>17</v>
-      </c>
-      <c r="C11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>18</v>
-      </c>
-      <c r="B12">
-        <v>18</v>
-      </c>
-      <c r="C12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>20</v>
-      </c>
-      <c r="B13">
-        <v>20</v>
-      </c>
-      <c r="C13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>22</v>
-      </c>
-      <c r="B14">
-        <v>22</v>
-      </c>
-      <c r="C14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>24</v>
-      </c>
-      <c r="B15">
-        <v>24</v>
-      </c>
-      <c r="C15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>27</v>
-      </c>
-      <c r="B16">
-        <v>27</v>
-      </c>
-      <c r="C16" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>29</v>
-      </c>
-      <c r="B17">
-        <v>29</v>
-      </c>
-      <c r="C17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>30</v>
-      </c>
-      <c r="B18">
-        <v>30</v>
-      </c>
-      <c r="C18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>31</v>
-      </c>
-      <c r="B19">
-        <v>31</v>
-      </c>
-      <c r="C19" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>34</v>
-      </c>
-      <c r="B20">
-        <v>34</v>
-      </c>
-      <c r="C20" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>35</v>
-      </c>
-      <c r="B21">
-        <v>35</v>
-      </c>
-      <c r="C21" t="s">
-        <v>21</v>
-      </c>
-      <c r="D21" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>36</v>
-      </c>
-      <c r="B22">
-        <v>36</v>
-      </c>
-      <c r="C22" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>38</v>
-      </c>
-      <c r="B23">
-        <v>38</v>
-      </c>
-      <c r="C23" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>39</v>
-      </c>
-      <c r="B24">
-        <v>39</v>
-      </c>
-      <c r="C24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>40</v>
-      </c>
-      <c r="B25">
-        <v>40</v>
-      </c>
-      <c r="C25" t="s">
-        <v>15</v>
-      </c>
-      <c r="D25" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>41</v>
-      </c>
-      <c r="B26">
-        <v>41</v>
-      </c>
-      <c r="C26" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>42</v>
-      </c>
-      <c r="B27">
-        <v>42</v>
-      </c>
-      <c r="C27" t="s">
-        <v>15</v>
-      </c>
-      <c r="D27" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>43</v>
-      </c>
-      <c r="B28">
-        <v>43</v>
-      </c>
-      <c r="C28" t="s">
-        <v>15</v>
-      </c>
-      <c r="D28" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>44</v>
-      </c>
-      <c r="B29">
-        <v>44</v>
-      </c>
-      <c r="C29" t="s">
-        <v>19</v>
-      </c>
-      <c r="D29" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>49</v>
-      </c>
-      <c r="B30">
-        <v>49</v>
-      </c>
-      <c r="C30" t="s">
-        <v>19</v>
-      </c>
-      <c r="D30" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>50</v>
-      </c>
-      <c r="B31">
-        <v>50</v>
-      </c>
-      <c r="C31" t="s">
-        <v>19</v>
-      </c>
-      <c r="D31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>51</v>
-      </c>
-      <c r="B32">
-        <v>51</v>
-      </c>
-      <c r="C32" t="s">
-        <v>19</v>
-      </c>
-      <c r="D32" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>53</v>
-      </c>
-      <c r="B33">
-        <v>53</v>
-      </c>
-      <c r="C33" t="s">
-        <v>19</v>
-      </c>
-      <c r="D33" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>57</v>
-      </c>
-      <c r="B34">
-        <v>57</v>
-      </c>
-      <c r="C34" t="s">
-        <v>21</v>
-      </c>
-      <c r="D34" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>58</v>
-      </c>
-      <c r="B35">
-        <v>58</v>
-      </c>
-      <c r="C35" t="s">
-        <v>19</v>
-      </c>
-      <c r="D35" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>59</v>
-      </c>
-      <c r="B36">
-        <v>59</v>
-      </c>
-      <c r="C36" t="s">
-        <v>19</v>
-      </c>
-      <c r="D36" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>63</v>
-      </c>
-      <c r="B37">
-        <v>63</v>
-      </c>
-      <c r="C37" t="s">
-        <v>13</v>
-      </c>
-      <c r="D37" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>64</v>
-      </c>
-      <c r="B38">
-        <v>64</v>
-      </c>
-      <c r="C38" t="s">
-        <v>15</v>
-      </c>
-      <c r="D38" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>65</v>
-      </c>
-      <c r="B39">
-        <v>65</v>
-      </c>
-      <c r="C39" t="s">
-        <v>15</v>
-      </c>
-      <c r="D39" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>67</v>
-      </c>
-      <c r="B40">
-        <v>67</v>
-      </c>
-      <c r="C40" t="s">
-        <v>19</v>
-      </c>
-      <c r="D40" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>68</v>
-      </c>
-      <c r="B41">
-        <v>68</v>
-      </c>
-      <c r="C41" t="s">
-        <v>13</v>
-      </c>
-      <c r="D41" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>69</v>
-      </c>
-      <c r="B42">
-        <v>69</v>
-      </c>
-      <c r="C42" t="s">
-        <v>13</v>
-      </c>
-      <c r="D42" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>71</v>
-      </c>
-      <c r="B43">
-        <v>71</v>
-      </c>
-      <c r="C43" t="s">
-        <v>19</v>
-      </c>
-      <c r="D43" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>74</v>
-      </c>
-      <c r="B44">
-        <v>74</v>
-      </c>
-      <c r="C44" t="s">
-        <v>13</v>
-      </c>
-      <c r="D44" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>75</v>
-      </c>
-      <c r="B45">
-        <v>75</v>
-      </c>
-      <c r="C45" t="s">
-        <v>19</v>
-      </c>
-      <c r="D45" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>77</v>
-      </c>
-      <c r="B46">
-        <v>77</v>
-      </c>
-      <c r="C46" t="s">
-        <v>15</v>
-      </c>
-      <c r="D46" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>83</v>
-      </c>
-      <c r="B47">
-        <v>83</v>
-      </c>
-      <c r="C47" t="s">
-        <v>21</v>
-      </c>
-      <c r="D47" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>86</v>
-      </c>
-      <c r="B48">
-        <v>86</v>
-      </c>
-      <c r="C48" t="s">
-        <v>15</v>
-      </c>
-      <c r="D48" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>88</v>
-      </c>
-      <c r="B49">
-        <v>88</v>
-      </c>
-      <c r="C49" t="s">
-        <v>13</v>
-      </c>
-      <c r="D49" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>89</v>
-      </c>
-      <c r="B50">
-        <v>89</v>
-      </c>
-      <c r="C50" t="s">
-        <v>19</v>
-      </c>
-      <c r="D50" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>91</v>
-      </c>
-      <c r="B51">
-        <v>91</v>
-      </c>
-      <c r="C51" t="s">
-        <v>15</v>
-      </c>
-      <c r="D51" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>92</v>
-      </c>
-      <c r="B52">
-        <v>92</v>
-      </c>
-      <c r="C52" t="s">
-        <v>19</v>
-      </c>
-      <c r="D52" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>94</v>
-      </c>
-      <c r="B53">
-        <v>94</v>
-      </c>
-      <c r="C53" t="s">
-        <v>15</v>
-      </c>
-      <c r="D53" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>95</v>
-      </c>
-      <c r="B54">
-        <v>95</v>
-      </c>
-      <c r="C54" t="s">
-        <v>11</v>
-      </c>
-      <c r="D54" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>96</v>
-      </c>
-      <c r="B55">
-        <v>96</v>
-      </c>
-      <c r="C55" t="s">
-        <v>15</v>
-      </c>
-      <c r="D55" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>99</v>
-      </c>
-      <c r="B56">
-        <v>99</v>
-      </c>
-      <c r="C56" t="s">
-        <v>19</v>
-      </c>
-      <c r="D56" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>100</v>
-      </c>
-      <c r="B57">
-        <v>100</v>
-      </c>
-      <c r="C57" t="s">
-        <v>21</v>
-      </c>
-      <c r="D57" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>101</v>
-      </c>
-      <c r="B58">
-        <v>101</v>
-      </c>
-      <c r="C58" t="s">
-        <v>13</v>
-      </c>
-      <c r="D58" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>105</v>
-      </c>
-      <c r="B59">
-        <v>105</v>
-      </c>
-      <c r="C59" t="s">
-        <v>19</v>
-      </c>
-      <c r="D59" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>107</v>
-      </c>
-      <c r="B60">
-        <v>107</v>
-      </c>
-      <c r="C60" t="s">
-        <v>15</v>
-      </c>
-      <c r="D60" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>113</v>
-      </c>
-      <c r="B61">
-        <v>113</v>
-      </c>
-      <c r="C61" t="s">
-        <v>19</v>
-      </c>
-      <c r="D61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>115</v>
-      </c>
-      <c r="B62">
-        <v>115</v>
-      </c>
-      <c r="C62" t="s">
-        <v>15</v>
-      </c>
-      <c r="D62" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <v>117</v>
-      </c>
-      <c r="B63">
-        <v>117</v>
-      </c>
-      <c r="C63" t="s">
-        <v>15</v>
-      </c>
-      <c r="D63" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>118</v>
-      </c>
-      <c r="B64">
-        <v>118</v>
-      </c>
-      <c r="C64" t="s">
-        <v>13</v>
-      </c>
-      <c r="D64" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>119</v>
-      </c>
-      <c r="B65">
-        <v>119</v>
-      </c>
-      <c r="C65" t="s">
-        <v>21</v>
-      </c>
-      <c r="D65" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <v>122</v>
-      </c>
-      <c r="B66">
-        <v>122</v>
-      </c>
-      <c r="C66" t="s">
-        <v>21</v>
-      </c>
-      <c r="D66" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67">
-        <v>124</v>
-      </c>
-      <c r="B67">
-        <v>124</v>
-      </c>
-      <c r="C67" t="s">
-        <v>21</v>
-      </c>
-      <c r="D67" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68">
-        <v>125</v>
-      </c>
-      <c r="B68">
-        <v>125</v>
-      </c>
-      <c r="C68" t="s">
-        <v>15</v>
-      </c>
-      <c r="D68" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69">
-        <v>126</v>
-      </c>
-      <c r="B69">
-        <v>126</v>
-      </c>
-      <c r="C69" t="s">
-        <v>21</v>
-      </c>
-      <c r="D69" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70">
-        <v>127</v>
-      </c>
-      <c r="B70">
-        <v>127</v>
-      </c>
-      <c r="C70" t="s">
-        <v>11</v>
-      </c>
-      <c r="D70" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71">
-        <v>128</v>
-      </c>
-      <c r="B71">
-        <v>128</v>
-      </c>
-      <c r="C71" t="s">
-        <v>15</v>
-      </c>
-      <c r="D71" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72">
-        <v>130</v>
-      </c>
-      <c r="B72">
-        <v>130</v>
-      </c>
-      <c r="C72" t="s">
-        <v>13</v>
-      </c>
-      <c r="D72" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73">
-        <v>131</v>
-      </c>
-      <c r="B73">
-        <v>131</v>
-      </c>
-      <c r="C73" t="s">
-        <v>13</v>
-      </c>
-      <c r="D73" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74">
-        <v>132</v>
-      </c>
-      <c r="B74">
-        <v>132</v>
-      </c>
-      <c r="C74" t="s">
-        <v>19</v>
-      </c>
-      <c r="D74" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <v>133</v>
-      </c>
-      <c r="B75">
-        <v>133</v>
-      </c>
-      <c r="C75" t="s">
-        <v>15</v>
-      </c>
-      <c r="D75" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76">
-        <v>134</v>
-      </c>
-      <c r="B76">
-        <v>134</v>
-      </c>
-      <c r="C76" t="s">
-        <v>15</v>
-      </c>
-      <c r="D76" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77">
-        <v>135</v>
-      </c>
-      <c r="B77">
-        <v>135</v>
-      </c>
-      <c r="C77" t="s">
-        <v>15</v>
-      </c>
-      <c r="D77" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78">
-        <v>137</v>
-      </c>
-      <c r="B78">
-        <v>137</v>
-      </c>
-      <c r="C78" t="s">
-        <v>13</v>
-      </c>
-      <c r="D78" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79">
-        <v>138</v>
-      </c>
-      <c r="B79">
-        <v>138</v>
-      </c>
-      <c r="C79" t="s">
-        <v>21</v>
-      </c>
-      <c r="D79" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80">
-        <v>141</v>
-      </c>
-      <c r="B80">
-        <v>141</v>
-      </c>
-      <c r="C80" t="s">
-        <v>15</v>
-      </c>
-      <c r="D80" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81">
-        <v>143</v>
-      </c>
-      <c r="B81">
-        <v>143</v>
-      </c>
-      <c r="C81" t="s">
-        <v>19</v>
-      </c>
-      <c r="D81" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82">
-        <v>145</v>
-      </c>
-      <c r="B82">
-        <v>145</v>
-      </c>
-      <c r="C82" t="s">
-        <v>19</v>
-      </c>
-      <c r="D82" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83">
-        <v>146</v>
-      </c>
-      <c r="B83">
-        <v>146</v>
-      </c>
-      <c r="C83" t="s">
-        <v>13</v>
-      </c>
-      <c r="D83" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84">
-        <v>147</v>
-      </c>
-      <c r="B84">
-        <v>147</v>
-      </c>
-      <c r="C84" t="s">
-        <v>19</v>
-      </c>
-      <c r="D84" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85">
-        <v>149</v>
-      </c>
-      <c r="B85">
-        <v>149</v>
-      </c>
-      <c r="C85" t="s">
-        <v>15</v>
-      </c>
-      <c r="D85" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86">
-        <v>154</v>
-      </c>
-      <c r="B86">
-        <v>154</v>
-      </c>
-      <c r="C86" t="s">
-        <v>15</v>
-      </c>
-      <c r="D86" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87">
-        <v>155</v>
-      </c>
-      <c r="B87">
-        <v>155</v>
-      </c>
-      <c r="C87" t="s">
-        <v>13</v>
-      </c>
-      <c r="D87" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88">
-        <v>156</v>
-      </c>
-      <c r="B88">
-        <v>156</v>
-      </c>
-      <c r="C88" t="s">
-        <v>19</v>
-      </c>
-      <c r="D88" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89">
-        <v>164</v>
-      </c>
-      <c r="B89">
-        <v>164</v>
-      </c>
-      <c r="C89" t="s">
-        <v>11</v>
-      </c>
-      <c r="D89" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90">
-        <v>165</v>
-      </c>
-      <c r="B90">
-        <v>165</v>
-      </c>
-      <c r="C90" t="s">
-        <v>15</v>
-      </c>
-      <c r="D90" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91">
-        <v>169</v>
-      </c>
-      <c r="B91">
-        <v>169</v>
-      </c>
-      <c r="C91" t="s">
-        <v>19</v>
-      </c>
-      <c r="D91" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92">
-        <v>171</v>
-      </c>
-      <c r="B92">
-        <v>171</v>
-      </c>
-      <c r="C92" t="s">
-        <v>19</v>
-      </c>
-      <c r="D92" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93">
-        <v>172</v>
-      </c>
-      <c r="B93">
-        <v>172</v>
-      </c>
-      <c r="C93" t="s">
-        <v>19</v>
-      </c>
-      <c r="D93" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94">
-        <v>174</v>
-      </c>
-      <c r="B94">
-        <v>174</v>
-      </c>
-      <c r="C94" t="s">
-        <v>15</v>
-      </c>
-      <c r="D94" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95">
-        <v>178</v>
-      </c>
-      <c r="B95">
-        <v>178</v>
-      </c>
-      <c r="C95" t="s">
-        <v>11</v>
-      </c>
-      <c r="D95" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96">
-        <v>179</v>
-      </c>
-      <c r="B96">
-        <v>179</v>
-      </c>
-      <c r="C96" t="s">
-        <v>19</v>
-      </c>
-      <c r="D96" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97">
-        <v>180</v>
-      </c>
-      <c r="B97">
-        <v>180</v>
-      </c>
-      <c r="C97" t="s">
-        <v>19</v>
-      </c>
-      <c r="D97" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98">
-        <v>182</v>
-      </c>
-      <c r="B98">
-        <v>182</v>
-      </c>
-      <c r="C98" t="s">
-        <v>15</v>
-      </c>
-      <c r="D98" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99">
-        <v>183</v>
-      </c>
-      <c r="B99">
-        <v>183</v>
-      </c>
-      <c r="C99" t="s">
-        <v>19</v>
-      </c>
-      <c r="D99" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100">
-        <v>184</v>
-      </c>
-      <c r="B100">
-        <v>184</v>
-      </c>
-      <c r="C100" t="s">
-        <v>11</v>
-      </c>
-      <c r="D100" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101">
-        <v>185</v>
-      </c>
-      <c r="B101">
-        <v>185</v>
-      </c>
-      <c r="C101" t="s">
-        <v>15</v>
-      </c>
-      <c r="D101" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102">
-        <v>186</v>
-      </c>
-      <c r="B102">
-        <v>186</v>
-      </c>
-      <c r="C102" t="s">
-        <v>19</v>
-      </c>
-      <c r="D102" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103">
-        <v>187</v>
-      </c>
-      <c r="B103">
-        <v>187</v>
-      </c>
-      <c r="C103" t="s">
-        <v>19</v>
-      </c>
-      <c r="D103" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104">
-        <v>191</v>
-      </c>
-      <c r="B104">
-        <v>191</v>
-      </c>
-      <c r="C104" t="s">
-        <v>15</v>
-      </c>
-      <c r="D104" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105">
-        <v>192</v>
-      </c>
-      <c r="B105">
-        <v>192</v>
-      </c>
-      <c r="C105" t="s">
-        <v>15</v>
-      </c>
-      <c r="D105" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106">
-        <v>194</v>
-      </c>
-      <c r="B106">
-        <v>194</v>
-      </c>
-      <c r="C106" t="s">
-        <v>11</v>
-      </c>
-      <c r="D106" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107">
-        <v>197</v>
-      </c>
-      <c r="B107">
-        <v>197</v>
-      </c>
-      <c r="C107" t="s">
-        <v>13</v>
-      </c>
-      <c r="D107" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108">
-        <v>199</v>
-      </c>
-      <c r="B108">
-        <v>199</v>
-      </c>
-      <c r="C108" t="s">
-        <v>15</v>
-      </c>
-      <c r="D108" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109">
-        <v>201</v>
-      </c>
-      <c r="B109">
-        <v>201</v>
-      </c>
-      <c r="C109" t="s">
-        <v>13</v>
-      </c>
-      <c r="D109" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110">
-        <v>206</v>
-      </c>
-      <c r="B110">
-        <v>206</v>
-      </c>
-      <c r="C110" t="s">
-        <v>15</v>
-      </c>
-      <c r="D110" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111">
-        <v>207</v>
-      </c>
-      <c r="B111">
-        <v>207</v>
-      </c>
-      <c r="C111" t="s">
-        <v>13</v>
-      </c>
-      <c r="D111" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112">
-        <v>208</v>
-      </c>
-      <c r="B112">
-        <v>208</v>
-      </c>
-      <c r="C112" t="s">
-        <v>19</v>
-      </c>
-      <c r="D112" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113">
-        <v>211</v>
-      </c>
-      <c r="B113">
-        <v>211</v>
-      </c>
-      <c r="C113" t="s">
-        <v>11</v>
-      </c>
-      <c r="D113" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114">
-        <v>213</v>
-      </c>
-      <c r="B114">
-        <v>213</v>
-      </c>
-      <c r="C114" t="s">
-        <v>19</v>
-      </c>
-      <c r="D114" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115">
-        <v>214</v>
-      </c>
-      <c r="B115">
-        <v>214</v>
-      </c>
-      <c r="C115" t="s">
-        <v>13</v>
-      </c>
-      <c r="D115" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116">
-        <v>215</v>
-      </c>
-      <c r="B116">
-        <v>215</v>
-      </c>
-      <c r="C116" t="s">
-        <v>15</v>
-      </c>
-      <c r="D116" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117">
-        <v>217</v>
-      </c>
-      <c r="B117">
-        <v>217</v>
-      </c>
-      <c r="C117" t="s">
-        <v>21</v>
-      </c>
-      <c r="D117" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118">
-        <v>218</v>
-      </c>
-      <c r="B118">
-        <v>218</v>
-      </c>
-      <c r="C118" t="s">
-        <v>19</v>
-      </c>
-      <c r="D118" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119">
-        <v>220</v>
-      </c>
-      <c r="B119">
-        <v>220</v>
-      </c>
-      <c r="C119" t="s">
-        <v>11</v>
-      </c>
-      <c r="D119" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120">
-        <v>223</v>
-      </c>
-      <c r="B120">
-        <v>223</v>
-      </c>
-      <c r="C120" t="s">
-        <v>15</v>
-      </c>
-      <c r="D120" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState ref="B2:D120">
-    <sortCondition ref="B1"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>